<commit_message>
#218 Gráfica rendimiento actualizada
</commit_message>
<xml_diff>
--- a/Conocimiento/Metodología/Gráfica rendimiento - desviaciones.xlsx
+++ b/Conocimiento/Metodología/Gráfica rendimiento - desviaciones.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19226"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{087B20E5-B272-413B-82E9-F7E7C9BD58FB}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB06C569-8FBE-487D-801D-7A917097F652}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -43,26 +43,26 @@
     <t>Álvaro Sánchez</t>
   </si>
   <si>
-    <t>ESTIMADO(TOTAL)</t>
-  </si>
-  <si>
     <t>Rendimiento</t>
   </si>
   <si>
     <t>Desviación</t>
   </si>
   <si>
-    <t>SP Estimados</t>
+    <t>Horas reales</t>
   </si>
   <si>
-    <t>SP Reales</t>
+    <t>SP Reales completados</t>
+  </si>
+  <si>
+    <t>SP Estimados (esta semana)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,8 +78,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -104,6 +111,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -114,10 +126,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -128,8 +141,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="12">
@@ -139,6 +157,13 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -165,10 +190,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -185,9 +206,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -247,36 +265,18 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="110"/>
+      <c14:style val="102"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="10"/>
+      <c:style val="2"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="es-ES" sz="3600"/>
-              <a:t>Overall performance</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -299,8 +299,12 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="212683"/>
+              <a:schemeClr val="accent1"/>
             </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
@@ -313,7 +317,7 @@
                   <a:p>
                     <a:r>
                       <a:rPr lang="en-US"/>
-                      <a:t>16</a:t>
+                      <a:t>109</a:t>
                     </a:r>
                   </a:p>
                 </c:rich>
@@ -328,7 +332,73 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000003-4A00-4472-AA0C-B05DF0A0FB03}"/>
+                  <c16:uniqueId val="{00000002-626D-48FD-BAE8-90C428035322}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="-2.3071155605613704E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000009-626D-48FD-BAE8-90C428035322}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.058201058200903E-3"/>
+                  <c:y val="-2.0973777823285186E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000A-626D-48FD-BAE8-90C428035322}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="-1.6779022258628151E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000B-626D-48FD-BAE8-90C428035322}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -340,11 +410,23 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr/>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="2000"/>
+                  <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
                 </a:pPr>
                 <a:endParaRPr lang="es-ES"/>
               </a:p>
@@ -399,172 +481,32 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>109</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>121</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100</c:v>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>87</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>100</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>100</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-4A00-4472-AA0C-B05DF0A0FB03}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Hoja1!$N$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Desviación</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:r>
-                      <a:rPr lang="en-US" sz="2000"/>
-                      <a:t>28</a:t>
-                    </a:r>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:dLblPos val="outEnd"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000006-4A00-4472-AA0C-B05DF0A0FB03}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="2000"/>
-                </a:pPr>
-                <a:endParaRPr lang="es-ES"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="0"/>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Hoja1!$L$2:$L$8</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>Alejandro Román</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Álvaro Domínguez</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Miguel Ángel Baños</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Alejandro Garrido</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Andrés Fernández</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Jesús Sosa</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Álvaro Sánchez</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Hoja1!$N$2:$N$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>71</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>50</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000007-4A00-4472-AA0C-B05DF0A0FB03}"/>
+              <c16:uniqueId val="{00000003-626D-48FD-BAE8-90C428035322}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -577,7 +519,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
         <c:axId val="200367104"/>
         <c:axId val="198023360"/>
       </c:barChart>
@@ -589,7 +532,7 @@
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="198023360"/>
@@ -606,17 +549,101 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:alpha val="71000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="3600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES" sz="3600" b="1"/>
+                  <a:t>Percentage</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="3600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
         <c:txPr>
-          <a:bodyPr/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="2600"/>
+              <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="es-ES"/>
           </a:p>
@@ -627,6 +654,10 @@
       </c:valAx>
       <c:spPr>
         <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
       </c:spPr>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
@@ -635,7 +666,22 @@
   </c:chart>
   <c:spPr>
     <a:noFill/>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
   </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -644,27 +690,570 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>619123</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>16327</xdr:rowOff>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>68034</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1319893</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>163286</xdr:rowOff>
+      <xdr:colOff>857250</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>27214</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
+        <xdr:cNvPr id="2" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63AB71D8-E782-449A-8184-FC22749F5ECA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9AA6EF00-EC4E-48D8-A04E-41A294C4F082}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -690,26 +1279,26 @@
   <autoFilter ref="A1:E8" xr:uid="{A9087340-591B-4F0F-AEB3-34D277FA196A}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{8F92CB3B-8B54-458E-8E49-3D3E92D320C6}" name="Miembro"/>
-    <tableColumn id="2" xr3:uid="{D8E5A923-47C9-4FE6-BFBA-0693C7A2FE5B}" name="SP Estimados" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{99F57447-8ACE-4D5E-993F-7638AD67D301}" name="SP Reales" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{2FEFB0C9-0244-4814-AE3B-A90686460067}" name="Desviación" dataDxfId="7">
+    <tableColumn id="2" xr3:uid="{D8E5A923-47C9-4FE6-BFBA-0693C7A2FE5B}" name="SP Estimados (esta semana)" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{99F57447-8ACE-4D5E-993F-7638AD67D301}" name="SP Reales completados" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{2FEFB0C9-0244-4814-AE3B-A90686460067}" name="Desviación" dataDxfId="3">
       <calculatedColumnFormula>(ABS(B2-C2)/B2)*100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{B2393DE2-1A0C-42B0-BEB6-ADD9E3920671}" name="ESTIMADO(TOTAL)" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{B2393DE2-1A0C-42B0-BEB6-ADD9E3920671}" name="Horas reales" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E9BC83C3-0DF0-43B6-9466-D863A1C25DB9}" name="Table3" displayName="Table3" ref="H1:J8" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E9BC83C3-0DF0-43B6-9466-D863A1C25DB9}" name="Table3" displayName="Table3" ref="H1:J8" totalsRowShown="0" headerRowDxfId="6">
   <autoFilter ref="H1:J8" xr:uid="{1DFF99CD-2980-4BCE-B37A-07AF8B606F33}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{D3D4D790-92D1-413E-913A-FBEE0E284042}" name="Miembro"/>
-    <tableColumn id="2" xr3:uid="{139AE897-522C-4DEC-A532-B72609CCE840}" name="Rendimiento" dataDxfId="0">
-      <calculatedColumnFormula>TRUNC((Table2[[#This Row],[SP Reales]]/(Table2[[#This Row],[SP Estimados]]))*100)</calculatedColumnFormula>
+    <tableColumn id="2" xr3:uid="{139AE897-522C-4DEC-A532-B72609CCE840}" name="Rendimiento" dataDxfId="1">
+      <calculatedColumnFormula>TRUNC((((Table2[[#This Row],[SP Reales completados]]/Table2[[#This Row],[SP Estimados (esta semana)]]) + ((Table2[[#This Row],[SP Reales completados]]/2)/Table2[[#This Row],[Horas reales]]))/2)*100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{FFBF626B-BAD2-4000-BE8B-DADC299A437F}" name="Desviación" dataDxfId="4">
+    <tableColumn id="3" xr3:uid="{FFBF626B-BAD2-4000-BE8B-DADC299A437F}" name="Desviación" dataDxfId="2">
       <calculatedColumnFormula>TRUNC(Table2[[#This Row],[Desviación]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -718,14 +1307,12 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{BAC02E39-CDE0-4808-916F-74679D9487F9}" name="Table35" displayName="Table35" ref="L1:N8" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{BAC02E39-CDE0-4808-916F-74679D9487F9}" name="Table35" displayName="Table35" ref="L1:N8" totalsRowShown="0" headerRowDxfId="5">
   <autoFilter ref="L1:N8" xr:uid="{0114544C-9B48-472A-987B-48CE0029F380}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{C653248D-3148-404A-B571-7DC19B3817A7}" name="Miembro"/>
-    <tableColumn id="2" xr3:uid="{228B0A4D-F7D1-422D-8C68-214AC76FAC6D}" name="Rendimiento" dataDxfId="2">
-      <calculatedColumnFormula>TRUNC((Table2[[#This Row],[SP Reales]]/(Table2[[#This Row],[SP Estimados]]/2))*100)</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="3" xr3:uid="{364A839A-72FB-4FBA-B1B9-50B180368C63}" name="Desviación" dataDxfId="1">
+    <tableColumn id="2" xr3:uid="{228B0A4D-F7D1-422D-8C68-214AC76FAC6D}" name="Rendimiento" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{364A839A-72FB-4FBA-B1B9-50B180368C63}" name="Desviación" dataDxfId="0">
       <calculatedColumnFormula>TRUNC(Table2[[#This Row],[Desviación]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -734,7 +1321,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1054,17 +1641,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.5703125" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="2" max="2" width="40" customWidth="1"/>
+    <col min="3" max="3" width="35.5703125" customWidth="1"/>
     <col min="4" max="4" width="17.140625" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
     <col min="8" max="8" width="22.42578125" customWidth="1"/>
@@ -1080,16 +1667,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>12</v>
-      </c>
       <c r="D1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>8</v>
       </c>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -1097,19 +1684,19 @@
         <v>0</v>
       </c>
       <c r="I1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>9</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>10</v>
       </c>
       <c r="L1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="M1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -1117,19 +1704,18 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <f>21</f>
-        <v>21</v>
+        <f>21/2</f>
+        <v>10.5</v>
       </c>
       <c r="C2" s="1">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D2" s="1">
         <f>(ABS(B2-C2)/B2)*100</f>
-        <v>71.428571428571431</v>
+        <v>23.809523809523807</v>
       </c>
       <c r="E2" s="1">
-        <f>Table2[[#This Row],[SP Estimados]]</f>
-        <v>21</v>
+        <v>6.77</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -1137,22 +1723,23 @@
         <v>1</v>
       </c>
       <c r="I2" s="1">
-        <f>TRUNC((Table2[[#This Row],[SP Reales]]/(Table2[[#This Row],[SP Estimados]]))*100)</f>
-        <v>28</v>
+        <f>TRUNC((((Table2[[#This Row],[SP Reales completados]]/Table2[[#This Row],[SP Estimados (esta semana)]]) + ((Table2[[#This Row],[SP Reales completados]]/2)/Table2[[#This Row],[Horas reales]]))/2)*100)</f>
+        <v>109</v>
       </c>
       <c r="J2" s="1">
         <f>TRUNC(Table2[[#This Row],[Desviación]])</f>
-        <v>71</v>
+        <v>23</v>
       </c>
       <c r="L2" t="s">
         <v>1</v>
       </c>
       <c r="M2" s="1">
-        <v>100</v>
+        <f>Table3[[#This Row],[Rendimiento]]</f>
+        <v>109</v>
       </c>
       <c r="N2" s="1">
         <f>TRUNC(Table2[[#This Row],[Desviación]])</f>
-        <v>71</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -1160,18 +1747,18 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
+        <f>24/2</f>
         <v>12</v>
       </c>
       <c r="C3" s="1">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1">
         <f t="shared" ref="D3:D8" si="0">(ABS(B3-C3)/B3)*100</f>
-        <v>50</v>
+        <v>8.3333333333333321</v>
       </c>
       <c r="E3" s="1">
-        <f>Table2[[#This Row],[SP Estimados]]</f>
-        <v>12</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
@@ -1179,23 +1766,23 @@
         <v>2</v>
       </c>
       <c r="I3" s="1">
-        <f>TRUNC((Table2[[#This Row],[SP Reales]]/(Table2[[#This Row],[SP Estimados]]))*100)</f>
-        <v>50</v>
+        <f>TRUNC((((Table2[[#This Row],[SP Reales completados]]/Table2[[#This Row],[SP Estimados (esta semana)]]) + ((Table2[[#This Row],[SP Reales completados]]/2)/Table2[[#This Row],[Horas reales]]))/2)*100)</f>
+        <v>121</v>
       </c>
       <c r="J3" s="1">
         <f>TRUNC(Table2[[#This Row],[Desviación]])</f>
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="L3" t="s">
         <v>2</v>
       </c>
       <c r="M3" s="1">
-        <f>TRUNC((Table2[[#This Row],[SP Reales]]/(Table2[[#This Row],[SP Estimados]]/2))*100)</f>
-        <v>100</v>
+        <f>Table3[[#This Row],[Rendimiento]]</f>
+        <v>121</v>
       </c>
       <c r="N3" s="1">
         <f>TRUNC(Table2[[#This Row],[Desviación]])</f>
-        <v>50</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -1206,15 +1793,14 @@
         <v>8</v>
       </c>
       <c r="C4" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D4" s="1">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="E4" s="1">
-        <f>Table2[[#This Row],[SP Estimados]]</f>
-        <v>8</v>
+        <v>6.33</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -1222,64 +1808,66 @@
         <v>3</v>
       </c>
       <c r="I4" s="1">
-        <f>TRUNC((Table2[[#This Row],[SP Reales]]/(Table2[[#This Row],[SP Estimados]]))*100)</f>
-        <v>75</v>
+        <f>TRUNC((((Table2[[#This Row],[SP Reales completados]]/Table2[[#This Row],[SP Estimados (esta semana)]]) + ((Table2[[#This Row],[SP Reales completados]]/2)/Table2[[#This Row],[Horas reales]]))/2)*100)</f>
+        <v>81</v>
       </c>
       <c r="J4" s="1">
         <f>TRUNC(Table2[[#This Row],[Desviación]])</f>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="L4" t="s">
         <v>3</v>
       </c>
       <c r="M4" s="1">
-        <v>100</v>
+        <f>Table3[[#This Row],[Rendimiento]]</f>
+        <v>81</v>
       </c>
       <c r="N4" s="1">
         <f>TRUNC(Table2[[#This Row],[Desviación]])</f>
-        <v>25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1">
-        <v>11</v>
-      </c>
-      <c r="C5" s="1">
-        <v>6</v>
-      </c>
-      <c r="D5" s="1">
+      <c r="B5" s="6">
+        <f>21/2</f>
+        <v>10.5</v>
+      </c>
+      <c r="C5" s="6">
+        <v>2</v>
+      </c>
+      <c r="D5" s="6">
         <f>(ABS(B5-C5)/B5)*100</f>
-        <v>45.454545454545453</v>
-      </c>
-      <c r="E5" s="1">
-        <f>Table2[[#This Row],[SP Estimados]]</f>
-        <v>11</v>
-      </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" t="s">
+        <v>80.952380952380949</v>
+      </c>
+      <c r="E5" s="6">
+        <v>1</v>
+      </c>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="1">
-        <f>TRUNC((Table2[[#This Row],[SP Reales]]/(Table2[[#This Row],[SP Estimados]]))*100)</f>
-        <v>54</v>
-      </c>
-      <c r="J5" s="1">
+      <c r="I5" s="6">
+        <f>TRUNC((((Table2[[#This Row],[SP Reales completados]]/Table2[[#This Row],[SP Estimados (esta semana)]]) + ((Table2[[#This Row],[SP Reales completados]]/2)/Table2[[#This Row],[Horas reales]]))/2)*100)</f>
+        <v>59</v>
+      </c>
+      <c r="J5" s="6">
         <f>TRUNC(Table2[[#This Row],[Desviación]])</f>
-        <v>45</v>
-      </c>
-      <c r="L5" t="s">
+        <v>80</v>
+      </c>
+      <c r="L5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="M5" s="1">
-        <v>100</v>
-      </c>
-      <c r="N5" s="1">
+      <c r="M5" s="6">
+        <f>Table3[[#This Row],[Rendimiento]]</f>
+        <v>59</v>
+      </c>
+      <c r="N5" s="6">
         <f>TRUNC(Table2[[#This Row],[Desviación]])</f>
-        <v>45</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -1287,19 +1875,18 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
+        <f>24/2</f>
         <v>12</v>
       </c>
       <c r="C6" s="1">
-        <f>2+9+1+1</f>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" s="1">
         <f>(ABS(B6-C6)/B6)*100</f>
-        <v>8.3333333333333321</v>
+        <v>0</v>
       </c>
       <c r="E6" s="1">
-        <f>Table2[[#This Row],[SP Estimados]]</f>
-        <v>12</v>
+        <v>6.57</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -1307,22 +1894,23 @@
         <v>5</v>
       </c>
       <c r="I6" s="1">
-        <f>TRUNC((Table2[[#This Row],[SP Reales]]/(Table2[[#This Row],[SP Estimados]]))*100)</f>
-        <v>108</v>
+        <f>TRUNC((((Table2[[#This Row],[SP Reales completados]]/Table2[[#This Row],[SP Estimados (esta semana)]]) + ((Table2[[#This Row],[SP Reales completados]]/2)/Table2[[#This Row],[Horas reales]]))/2)*100)</f>
+        <v>95</v>
       </c>
       <c r="J6" s="1">
         <f>TRUNC(Table2[[#This Row],[Desviación]])</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="L6" t="s">
         <v>5</v>
       </c>
       <c r="M6" s="1">
-        <v>87</v>
+        <f>Table3[[#This Row],[Rendimiento]]</f>
+        <v>95</v>
       </c>
       <c r="N6" s="1">
         <f>TRUNC(Table2[[#This Row],[Desviación]])</f>
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -1330,18 +1918,18 @@
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>10</v>
+        <f>24/2</f>
+        <v>12</v>
       </c>
       <c r="C7" s="1">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D7" s="1">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="E7" s="1">
-        <f>Table2[[#This Row],[SP Estimados]]</f>
-        <v>10</v>
+        <v>6.55</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
@@ -1349,22 +1937,23 @@
         <v>6</v>
       </c>
       <c r="I7" s="1">
-        <f>TRUNC((Table2[[#This Row],[SP Reales]]/(Table2[[#This Row],[SP Estimados]]))*100)</f>
-        <v>60</v>
+        <f>TRUNC((((Table2[[#This Row],[SP Reales completados]]/Table2[[#This Row],[SP Estimados (esta semana)]]) + ((Table2[[#This Row],[SP Reales completados]]/2)/Table2[[#This Row],[Horas reales]]))/2)*100)</f>
+        <v>95</v>
       </c>
       <c r="J7" s="1">
         <f>TRUNC(Table2[[#This Row],[Desviación]])</f>
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="L7" t="s">
         <v>6</v>
       </c>
       <c r="M7" s="1">
-        <v>100</v>
+        <f>Table3[[#This Row],[Rendimiento]]</f>
+        <v>95</v>
       </c>
       <c r="N7" s="1">
         <f>TRUNC(Table2[[#This Row],[Desviación]])</f>
-        <v>40</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -1372,18 +1961,17 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="1">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D8" s="1">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E8" s="1">
-        <f>Table2[[#This Row],[SP Estimados]]</f>
-        <v>12</v>
+        <v>5.67</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
@@ -1391,24 +1979,27 @@
         <v>7</v>
       </c>
       <c r="I8" s="1">
-        <f>TRUNC((Table2[[#This Row],[SP Reales]]/(Table2[[#This Row],[SP Estimados]]))*100)</f>
-        <v>50</v>
+        <f>TRUNC((((Table2[[#This Row],[SP Reales completados]]/Table2[[#This Row],[SP Estimados (esta semana)]]) + ((Table2[[#This Row],[SP Reales completados]]/2)/Table2[[#This Row],[Horas reales]]))/2)*100)</f>
+        <v>98</v>
       </c>
       <c r="J8" s="1">
         <f>TRUNC(Table2[[#This Row],[Desviación]])</f>
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="L8" t="s">
         <v>7</v>
       </c>
       <c r="M8" s="1">
-        <f>TRUNC((Table2[[#This Row],[SP Reales]]/(Table2[[#This Row],[SP Estimados]]/2))*100)</f>
-        <v>100</v>
+        <f>Table3[[#This Row],[Rendimiento]]</f>
+        <v>98</v>
       </c>
       <c r="N8" s="1">
         <f>TRUNC(Table2[[#This Row],[Desviación]])</f>
-        <v>50</v>
-      </c>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I9" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1428,7 +2019,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1440,7 +2031,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>